<commit_message>
Modified mapping function to pass mapping test
</commit_message>
<xml_diff>
--- a/ourClueLayout.xlsx
+++ b/ourClueLayout.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jake\Desktop\Folders\CSCI306\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edgar\workspace\ClueGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -253,6 +253,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -288,6 +305,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -446,15 +480,15 @@
       <selection activeCell="Y16" sqref="Y16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="2.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.109375" customWidth="1"/>
-    <col min="9" max="10" width="2.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="7" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.140625" customWidth="1"/>
+    <col min="9" max="10" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="23" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -525,7 +559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -596,7 +630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -667,7 +701,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -738,7 +772,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -809,7 +843,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -880,7 +914,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -951,7 +985,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1022,7 +1056,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -1093,7 +1127,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1164,7 +1198,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -1235,7 +1269,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -1306,7 +1340,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
@@ -1377,7 +1411,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
@@ -1448,7 +1482,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
@@ -1519,7 +1553,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -1590,7 +1624,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -1661,7 +1695,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
@@ -1732,7 +1766,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>5</v>
       </c>
@@ -1803,7 +1837,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>5</v>
       </c>
@@ -1874,7 +1908,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>5</v>
       </c>
@@ -1945,7 +1979,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>5</v>
       </c>
@@ -2016,7 +2050,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0</v>
       </c>

</xml_diff>